<commit_message>
replica location table, another experiment
git-svn-id: file://localhost/tmp/svn2git/svn@2992 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/replica_location.xlsx
+++ b/papers/async-re/data/replica_location.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28640" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14300" windowHeight="11800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
   <si>
     <t>Replicas 0-3 on QB</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t>The BigJobs started within 3 minutes of each other</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Experiment #58, Async-Cent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The BigJobs started within 2 minutes of each other</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -88,6 +100,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -118,8 +136,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="D128" sqref="D128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1295,9 +1316,396 @@
         <v>15</v>
       </c>
     </row>
+    <row r="89" spans="1:4">
+      <c r="A89" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
+        <v>2</v>
+      </c>
+      <c r="B91" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93">
+        <v>1</v>
+      </c>
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94">
+        <v>2</v>
+      </c>
+      <c r="B94">
+        <v>3</v>
+      </c>
+      <c r="C94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95">
+        <v>3</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96">
+        <v>4</v>
+      </c>
+      <c r="B96">
+        <v>3</v>
+      </c>
+      <c r="C96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97">
+        <v>5</v>
+      </c>
+      <c r="B97">
+        <v>5</v>
+      </c>
+      <c r="C97">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98">
+        <v>6</v>
+      </c>
+      <c r="B98">
+        <v>6</v>
+      </c>
+      <c r="C98">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99">
+        <v>7</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100">
+        <v>8</v>
+      </c>
+      <c r="B100">
+        <v>3</v>
+      </c>
+      <c r="C100">
+        <v>2</v>
+      </c>
+      <c r="D100" s="1"/>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101">
+        <v>9</v>
+      </c>
+      <c r="B101">
+        <v>4</v>
+      </c>
+      <c r="C101">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102">
+        <v>10</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103">
+        <v>11</v>
+      </c>
+      <c r="B103">
+        <v>2</v>
+      </c>
+      <c r="C103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104">
+        <v>12</v>
+      </c>
+      <c r="B104">
+        <v>6</v>
+      </c>
+      <c r="C104">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105">
+        <v>13</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106">
+        <v>14</v>
+      </c>
+      <c r="B106">
+        <v>4</v>
+      </c>
+      <c r="C106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107">
+        <v>15</v>
+      </c>
+      <c r="B107">
+        <v>3</v>
+      </c>
+      <c r="C107">
+        <v>5</v>
+      </c>
+      <c r="D107" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108">
+        <v>16</v>
+      </c>
+      <c r="B108">
+        <v>6</v>
+      </c>
+      <c r="C108">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109">
+        <v>17</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110">
+        <v>18</v>
+      </c>
+      <c r="B110">
+        <v>3</v>
+      </c>
+      <c r="C110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111">
+        <v>19</v>
+      </c>
+      <c r="B111">
+        <v>4</v>
+      </c>
+      <c r="C111">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112">
+        <v>20</v>
+      </c>
+      <c r="B112">
+        <v>6</v>
+      </c>
+      <c r="C112">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113">
+        <v>21</v>
+      </c>
+      <c r="B113">
+        <v>3</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114">
+        <v>22</v>
+      </c>
+      <c r="B114">
+        <v>2</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115">
+        <v>23</v>
+      </c>
+      <c r="B115">
+        <v>4</v>
+      </c>
+      <c r="C115">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116">
+        <v>24</v>
+      </c>
+      <c r="B116">
+        <v>6</v>
+      </c>
+      <c r="C116">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117">
+        <v>25</v>
+      </c>
+      <c r="B117">
+        <v>3</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118">
+        <v>26</v>
+      </c>
+      <c r="B118">
+        <v>2</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119">
+        <v>27</v>
+      </c>
+      <c r="B119">
+        <v>4</v>
+      </c>
+      <c r="C119">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120">
+        <v>28</v>
+      </c>
+      <c r="B120">
+        <v>6</v>
+      </c>
+      <c r="C120">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121">
+        <v>29</v>
+      </c>
+      <c r="B121">
+        <v>3</v>
+      </c>
+      <c r="C121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122">
+        <v>30</v>
+      </c>
+      <c r="B122">
+        <v>2</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123">
+        <v>31</v>
+      </c>
+      <c r="B123">
+        <v>4</v>
+      </c>
+      <c r="C123">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124">
+        <v>32</v>
+      </c>
+      <c r="B124">
+        <v>6</v>
+      </c>
+      <c r="C124">
+        <v>0</v>
+      </c>
+      <c r="D124" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" t="s">
+        <v>13</v>
+      </c>
+      <c r="D127" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>